<commit_message>
upload hrsimul excel file2
</commit_message>
<xml_diff>
--- a/data/hrdata.xlsx
+++ b/data/hrdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byeun\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3259F5F-69AB-43D8-A54E-B605ED168453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580CAB3-0117-48D1-A3F0-757922DA9914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20020" yWindow="160" windowWidth="22980" windowHeight="20740" xr2:uid="{475C43B0-F245-4777-8801-15C7C5FC6444}"/>
   </bookViews>
   <sheets>
-    <sheet name="date" sheetId="3" r:id="rId1"/>
+    <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="data_template" sheetId="1" r:id="rId2"/>
     <sheet name="lookup" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -487,7 +487,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J42" sqref="J41:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3473,11 +3473,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C2" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -3485,23 +3485,23 @@
       </c>
       <c r="E2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H2" s="1">
         <f ca="1">RANDBETWEEN(DATE(2010,1,1), DATE(2022,8,1))</f>
-        <v>41392</v>
-      </c>
-      <c r="I2" s="1">
+        <v>44021</v>
+      </c>
+      <c r="I2" s="1" t="str">
         <f ca="1">IF(E2="계약직", RANDBETWEEN(DATE(2023,2,1), DATE(2026,12,1)), "")</f>
-        <v>45009</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3515,11 +3515,11 @@
       </c>
       <c r="C3" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>가급</v>
       </c>
       <c r="E3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -3527,19 +3527,19 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H66" ca="1" si="0">RANDBETWEEN(DATE(2010,1,1), DATE(2022,8,1))</f>
-        <v>44486</v>
+        <v>43713</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I66" ca="1" si="1">IF(E3="계약직", RANDBETWEEN(DATE(2023,2,1), DATE(2026,12,1)), "")</f>
-        <v>46281</v>
+        <v>45498</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3557,11 +3557,11 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E4" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F4" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -3573,11 +3573,11 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43441</v>
-      </c>
-      <c r="I4" s="1">
+        <v>40946</v>
+      </c>
+      <c r="I4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45833</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3603,15 +3603,15 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44188</v>
+        <v>42626</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="D6" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -3641,15 +3641,15 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>채권관리부</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43153</v>
+        <v>43357</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3659,7 +3659,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="C7" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="E7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -3683,21 +3683,21 @@
       </c>
       <c r="G7" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40676</v>
-      </c>
-      <c r="I7" s="1">
+        <v>42413</v>
+      </c>
+      <c r="I7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45376</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -3705,15 +3705,15 @@
       </c>
       <c r="C8" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>마급</v>
       </c>
       <c r="E8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -3721,21 +3721,21 @@
       </c>
       <c r="G8" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42650</v>
-      </c>
-      <c r="I8" s="1">
+        <v>41159</v>
+      </c>
+      <c r="I8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45193</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B9" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43333</v>
+        <v>43072</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3789,23 +3789,23 @@
       </c>
       <c r="E10" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>홍보실</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42132</v>
-      </c>
-      <c r="I10" s="1" t="str">
+        <v>42542</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45178</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -3823,7 +3823,7 @@
       </c>
       <c r="D11" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>나급</v>
       </c>
       <c r="E11" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -3835,15 +3835,15 @@
       </c>
       <c r="G11" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40783</v>
+        <v>43753</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>46276</v>
+        <v>45294</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="E12" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F12" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -3873,33 +3873,33 @@
       </c>
       <c r="G12" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41561</v>
-      </c>
-      <c r="I12" s="1" t="str">
+        <v>43026</v>
+      </c>
+      <c r="I12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>46267</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B13" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>32874</v>
       </c>
       <c r="D13" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E13" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -3911,11 +3911,11 @@
       </c>
       <c r="G13" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43592</v>
+        <v>41315</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="B14" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C14" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="D14" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>다급</v>
       </c>
       <c r="E14" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -3949,11 +3949,11 @@
       </c>
       <c r="G14" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42458</v>
+        <v>43339</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3963,15 +3963,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B15" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>32874</v>
       </c>
       <c r="D15" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43136</v>
+        <v>43571</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4001,7 +4001,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B16" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="D16" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>나급</v>
       </c>
       <c r="E16" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43092</v>
+        <v>44548</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4051,27 +4051,27 @@
       </c>
       <c r="D17" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>마급</v>
       </c>
       <c r="E17" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F17" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40775</v>
-      </c>
-      <c r="I17" s="1">
+        <v>44612</v>
+      </c>
+      <c r="I17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45024</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="D18" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>다급</v>
       </c>
       <c r="E18" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4101,11 +4101,11 @@
       </c>
       <c r="G18" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41476</v>
+        <v>40294</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="B19" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="D19" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>나급</v>
       </c>
       <c r="E19" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4139,11 +4139,11 @@
       </c>
       <c r="G19" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43187</v>
+        <v>42045</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4153,7 +4153,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4161,11 +4161,11 @@
       </c>
       <c r="C20" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D20" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>라급</v>
       </c>
       <c r="E20" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4177,11 +4177,11 @@
       </c>
       <c r="G20" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43218</v>
+        <v>43299</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4191,7 +4191,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B21" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4199,15 +4199,15 @@
       </c>
       <c r="C21" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D21" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>가급</v>
       </c>
       <c r="E21" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F21" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4219,11 +4219,11 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41499</v>
-      </c>
-      <c r="I21" s="1">
+        <v>44170</v>
+      </c>
+      <c r="I21" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45947</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -4241,11 +4241,11 @@
       </c>
       <c r="D22" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E22" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F22" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4253,15 +4253,15 @@
       </c>
       <c r="G22" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41624</v>
-      </c>
-      <c r="I22" s="1" t="str">
+        <v>42628</v>
+      </c>
+      <c r="I22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45587</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -4275,41 +4275,41 @@
       </c>
       <c r="C23" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D23" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E23" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F23" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43094</v>
-      </c>
-      <c r="I23" s="1" t="str">
+        <v>42347</v>
+      </c>
+      <c r="I23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45919</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B24" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C24" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="E24" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F24" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4333,11 +4333,11 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44660</v>
-      </c>
-      <c r="I24" s="1" t="str">
+        <v>41265</v>
+      </c>
+      <c r="I24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45445</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -4355,33 +4355,33 @@
       </c>
       <c r="D25" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>다급</v>
       </c>
       <c r="E25" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F25" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>홍보실</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43035</v>
-      </c>
-      <c r="I25" s="1" t="str">
+        <v>43253</v>
+      </c>
+      <c r="I25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45944</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4389,11 +4389,11 @@
       </c>
       <c r="C26" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>마급</v>
       </c>
       <c r="E26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4401,15 +4401,15 @@
       </c>
       <c r="F26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41059</v>
+        <v>43019</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4423,19 +4423,19 @@
       </c>
       <c r="B27" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D27" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>마급</v>
       </c>
       <c r="E27" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F27" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4443,15 +4443,15 @@
       </c>
       <c r="G27" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44227</v>
-      </c>
-      <c r="I27" s="1" t="str">
+        <v>42833</v>
+      </c>
+      <c r="I27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45266</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -4465,15 +4465,15 @@
       </c>
       <c r="C28" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D28" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E28" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F28" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4481,15 +4481,15 @@
       </c>
       <c r="G28" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41221</v>
-      </c>
-      <c r="I28" s="1" t="str">
+        <v>41777</v>
+      </c>
+      <c r="I28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45769</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -4503,11 +4503,11 @@
       </c>
       <c r="C29" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>29221</v>
       </c>
       <c r="D29" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E29" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4519,11 +4519,11 @@
       </c>
       <c r="G29" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40446</v>
+        <v>41674</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4537,19 +4537,19 @@
       </c>
       <c r="B30" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C30" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D30" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>다급</v>
       </c>
       <c r="E30" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F30" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4557,21 +4557,21 @@
       </c>
       <c r="G30" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42052</v>
-      </c>
-      <c r="I30" s="1">
+        <v>42596</v>
+      </c>
+      <c r="I30" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45290</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="C31" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -4587,63 +4587,63 @@
       </c>
       <c r="E31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41771</v>
-      </c>
-      <c r="I31" s="1" t="str">
+        <v>42907</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>46212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C32" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>마급</v>
+      </c>
+      <c r="E32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>홍보실</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>41828</v>
+      </c>
+      <c r="I32" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C32" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
-      </c>
-      <c r="D32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
-      </c>
-      <c r="G32" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
-      </c>
-      <c r="H32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>40902</v>
-      </c>
-      <c r="I32" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>46178</v>
-      </c>
-    </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="C33" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D33" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -4671,11 +4671,11 @@
       </c>
       <c r="G33" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42250</v>
+        <v>40916</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4693,15 +4693,15 @@
       </c>
       <c r="C34" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D34" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>라급</v>
       </c>
       <c r="E34" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F34" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4709,25 +4709,25 @@
       </c>
       <c r="G34" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42281</v>
-      </c>
-      <c r="I34" s="1">
+        <v>40636</v>
+      </c>
+      <c r="I34" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>46195</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C35" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -4735,103 +4735,103 @@
       </c>
       <c r="D35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>다급</v>
       </c>
       <c r="E35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G35" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42458</v>
-      </c>
-      <c r="I35" s="1" t="str">
+        <v>44755</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>45825</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C36" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>25569</v>
+      </c>
+      <c r="D36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>나급</v>
+      </c>
+      <c r="E36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>금융연구부</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>41338</v>
+      </c>
+      <c r="I36" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
-      </c>
-      <c r="C36" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
-      </c>
-      <c r="D36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G36" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
-      </c>
-      <c r="H36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>41438</v>
-      </c>
-      <c r="I36" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>46070</v>
-      </c>
-    </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C37" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>가급</v>
       </c>
       <c r="E37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40322</v>
-      </c>
-      <c r="I37" s="1">
+        <v>43286</v>
+      </c>
+      <c r="I37" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45219</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -4849,11 +4849,11 @@
       </c>
       <c r="D38" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>라급</v>
       </c>
       <c r="E38" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F38" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -4861,21 +4861,21 @@
       </c>
       <c r="G38" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42186</v>
-      </c>
-      <c r="I38" s="1">
+        <v>40682</v>
+      </c>
+      <c r="I38" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45427</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B39" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="D39" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E39" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4899,11 +4899,11 @@
       </c>
       <c r="G39" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42388</v>
+        <v>41255</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4917,41 +4917,41 @@
       </c>
       <c r="B40" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C40" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D40" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>나급</v>
       </c>
       <c r="E40" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F40" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40303</v>
-      </c>
-      <c r="I40" s="1">
+        <v>41634</v>
+      </c>
+      <c r="I40" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45772</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B41" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -4959,11 +4959,11 @@
       </c>
       <c r="C41" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D41" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>라급</v>
       </c>
       <c r="E41" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -4975,11 +4975,11 @@
       </c>
       <c r="G41" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43062</v>
+        <v>41768</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4989,23 +4989,23 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B42" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C42" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D42" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E42" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F42" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5017,11 +5017,11 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43786</v>
-      </c>
-      <c r="I42" s="1" t="str">
+        <v>44043</v>
+      </c>
+      <c r="I42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>46254</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -5035,11 +5035,11 @@
       </c>
       <c r="C43" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>32874</v>
       </c>
       <c r="D43" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E43" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5051,11 +5051,11 @@
       </c>
       <c r="G43" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44488</v>
+        <v>40236</v>
       </c>
       <c r="I43" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5065,7 +5065,7 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -5073,11 +5073,11 @@
       </c>
       <c r="C44" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="F44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G44" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42553</v>
+        <v>40952</v>
       </c>
       <c r="I44" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B45" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C45" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="D45" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>가급</v>
       </c>
       <c r="E45" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5123,15 +5123,15 @@
       </c>
       <c r="F45" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G45" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40360</v>
+        <v>40601</v>
       </c>
       <c r="I45" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="E46" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F46" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5169,51 +5169,51 @@
       </c>
       <c r="H46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41954</v>
-      </c>
-      <c r="I46" s="1" t="str">
+        <v>43391</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>46228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>여</v>
+      </c>
+      <c r="B47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C47" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>나급</v>
+      </c>
+      <c r="E47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>연구분석부</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44448</v>
+      </c>
+      <c r="I47" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C47" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
-      </c>
-      <c r="D47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
-      </c>
-      <c r="G47" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
-      </c>
-      <c r="H47" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>40960</v>
-      </c>
-      <c r="I47" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>46200</v>
-      </c>
-    </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
@@ -5229,11 +5229,11 @@
       </c>
       <c r="D48" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>마급</v>
       </c>
       <c r="E48" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F48" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5241,33 +5241,33 @@
       </c>
       <c r="G48" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42341</v>
-      </c>
-      <c r="I48" s="1">
+        <v>40949</v>
+      </c>
+      <c r="I48" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>46039</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C49" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5275,15 +5275,15 @@
       </c>
       <c r="F49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G49" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42756</v>
+        <v>41992</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5293,7 +5293,7 @@
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B50" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -5301,11 +5301,11 @@
       </c>
       <c r="C50" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>다급</v>
       </c>
       <c r="E50" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5317,15 +5317,15 @@
       </c>
       <c r="G50" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44421</v>
+        <v>41931</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>46212</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="E51" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F51" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5355,169 +5355,169 @@
       </c>
       <c r="G51" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>연구분석부</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42353</v>
-      </c>
-      <c r="I51" s="1" t="str">
+        <v>42002</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>45099</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C52" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>25569</v>
+      </c>
+      <c r="D52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>나급</v>
+      </c>
+      <c r="E52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>계약직</v>
+      </c>
+      <c r="F52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>재산관리부</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>41273</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>여</v>
+      </c>
+      <c r="B53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C53" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>다급</v>
+      </c>
+      <c r="E53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>계약직</v>
+      </c>
+      <c r="F53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>팀장</v>
+      </c>
+      <c r="G53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>재산관리부</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>40294</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>46047</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C54" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>다급</v>
+      </c>
+      <c r="E54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>채권관리부</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>40736</v>
+      </c>
+      <c r="I54" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B52" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C52" s="1">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>여</v>
+      </c>
+      <c r="B55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>스위스</v>
+      </c>
+      <c r="C55" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
         <v>29221</v>
       </c>
-      <c r="D52" t="str">
+      <c r="D55" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
         <v>다급</v>
       </c>
-      <c r="E52" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F52" t="str">
+      <c r="E55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F55" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
         <v>사원</v>
       </c>
-      <c r="G52" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
-      </c>
-      <c r="H52" s="1">
+      <c r="G55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>재산관리부</v>
+      </c>
+      <c r="H55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41220</v>
-      </c>
-      <c r="I52" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>45643</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C53" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
-      </c>
-      <c r="D53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
-      </c>
-      <c r="F53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G53" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
-      </c>
-      <c r="H53" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>41179</v>
-      </c>
-      <c r="I53" s="1" t="str">
+        <v>42108</v>
+      </c>
+      <c r="I55" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
-      </c>
-      <c r="B54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
-      </c>
-      <c r="C54" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
-      </c>
-      <c r="D54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
-      </c>
-      <c r="E54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G54" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
-      </c>
-      <c r="H54" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43894</v>
-      </c>
-      <c r="I54" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>46149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
-      </c>
-      <c r="B55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C55" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
-      </c>
-      <c r="D55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
-      </c>
-      <c r="E55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G55" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
-      </c>
-      <c r="H55" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44095</v>
-      </c>
-      <c r="I55" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>46070</v>
-      </c>
-    </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
@@ -5525,15 +5525,15 @@
       </c>
       <c r="B56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C56" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>라급</v>
       </c>
       <c r="E56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5541,15 +5541,15 @@
       </c>
       <c r="F56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G56" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41671</v>
+        <v>41682</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5567,11 +5567,11 @@
       </c>
       <c r="C57" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D57" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>가급</v>
       </c>
       <c r="E57" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5583,11 +5583,11 @@
       </c>
       <c r="G57" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44549</v>
+        <v>44619</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5601,15 +5601,15 @@
       </c>
       <c r="B58" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C58" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D58" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>마급</v>
       </c>
       <c r="E58" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41517</v>
+        <v>41016</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5643,15 +5643,15 @@
       </c>
       <c r="C59" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>마급</v>
       </c>
       <c r="E59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5659,15 +5659,15 @@
       </c>
       <c r="G59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44603</v>
-      </c>
-      <c r="I59" s="1">
+        <v>40497</v>
+      </c>
+      <c r="I59" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>45442</v>
+        <v/>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -5681,11 +5681,11 @@
       </c>
       <c r="C60" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D60" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E60" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5697,15 +5697,15 @@
       </c>
       <c r="G60" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43706</v>
+        <v>41682</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45348</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -5715,7 +5715,7 @@
       </c>
       <c r="B61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C61" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -5723,7 +5723,7 @@
       </c>
       <c r="D61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5735,11 +5735,11 @@
       </c>
       <c r="G61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42007</v>
+        <v>41221</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5757,11 +5757,11 @@
       </c>
       <c r="C62" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D62" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>마급</v>
       </c>
       <c r="E62" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5769,15 +5769,15 @@
       </c>
       <c r="F62" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G62" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44531</v>
+        <v>41708</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5795,37 +5795,37 @@
       </c>
       <c r="C63" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D63" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E63" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F63" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G63" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>홍보실</v>
       </c>
       <c r="H63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41382</v>
-      </c>
-      <c r="I63" s="1" t="str">
+        <v>42978</v>
+      </c>
+      <c r="I63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>45343</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -5833,15 +5833,15 @@
       </c>
       <c r="C64" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>가급</v>
       </c>
       <c r="E64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -5849,15 +5849,15 @@
       </c>
       <c r="G64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40717</v>
-      </c>
-      <c r="I64" s="1" t="str">
+        <v>43632</v>
+      </c>
+      <c r="I64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>46311</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -5871,11 +5871,11 @@
       </c>
       <c r="C65" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D65" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E65" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5887,11 +5887,11 @@
       </c>
       <c r="G65" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40733</v>
+        <v>43315</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="B66" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C66" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -5921,15 +5921,15 @@
       </c>
       <c r="F66" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G66" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41522</v>
+        <v>43764</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5939,7 +5939,7 @@
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="D67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>나급</v>
       </c>
       <c r="E67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -5963,15 +5963,15 @@
       </c>
       <c r="G67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H67" s="1">
         <f t="shared" ref="H67:H101" ca="1" si="2">RANDBETWEEN(DATE(2010,1,1), DATE(2022,8,1))</f>
-        <v>40612</v>
+        <v>41331</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" ref="I67:I101" ca="1" si="3">IF(E67="계약직", RANDBETWEEN(DATE(2023,2,1), DATE(2026,12,1)), "")</f>
-        <v>45898</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -5985,15 +5985,15 @@
       </c>
       <c r="C68" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>마급</v>
       </c>
       <c r="E68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6001,21 +6001,21 @@
       </c>
       <c r="G68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>채권관리부</v>
       </c>
       <c r="H68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40183</v>
-      </c>
-      <c r="I68" s="1" t="str">
+        <v>40248</v>
+      </c>
+      <c r="I68" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>45754</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="D69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>나급</v>
       </c>
       <c r="E69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6035,15 +6035,15 @@
       </c>
       <c r="F69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40237</v>
+        <v>41968</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C70" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="D70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>다급</v>
       </c>
       <c r="E70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="F70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43287</v>
+        <v>42240</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6091,7 +6091,7 @@
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6103,7 +6103,7 @@
       </c>
       <c r="D71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>라급</v>
       </c>
       <c r="E71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6111,15 +6111,15 @@
       </c>
       <c r="F71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G71" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>채권관리부</v>
       </c>
       <c r="H71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40869</v>
+        <v>40571</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6129,19 +6129,19 @@
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C72" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>다급</v>
       </c>
       <c r="E72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6149,7 +6149,7 @@
       </c>
       <c r="F72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G72" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43385</v>
+        <v>40415</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6167,15 +6167,15 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C73" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -6183,7 +6183,7 @@
       </c>
       <c r="E73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6191,21 +6191,21 @@
       </c>
       <c r="G73" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>42595</v>
-      </c>
-      <c r="I73" s="1">
+        <v>43805</v>
+      </c>
+      <c r="I73" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>45590</v>
+        <v/>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B74" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6213,15 +6213,15 @@
       </c>
       <c r="C74" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D74" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>가급</v>
       </c>
       <c r="E74" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F74" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6233,11 +6233,11 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43441</v>
-      </c>
-      <c r="I74" s="1" t="str">
+        <v>40345</v>
+      </c>
+      <c r="I74" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>45820</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -6251,15 +6251,15 @@
       </c>
       <c r="C75" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>32874</v>
       </c>
       <c r="D75" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E75" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F75" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6267,15 +6267,15 @@
       </c>
       <c r="G75" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43150</v>
-      </c>
-      <c r="I75" s="1" t="str">
+        <v>44582</v>
+      </c>
+      <c r="I75" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>45867</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -6285,19 +6285,19 @@
       </c>
       <c r="B76" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C76" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>29221</v>
       </c>
       <c r="D76" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>다급</v>
       </c>
       <c r="E76" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F76" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6305,21 +6305,21 @@
       </c>
       <c r="G76" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>홍보실</v>
       </c>
       <c r="H76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41684</v>
-      </c>
-      <c r="I76" s="1" t="str">
+        <v>41936</v>
+      </c>
+      <c r="I76" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>45597</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B77" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6327,11 +6327,11 @@
       </c>
       <c r="C77" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>32874</v>
       </c>
       <c r="D77" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>가급</v>
       </c>
       <c r="E77" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="H77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44556</v>
+        <v>44589</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6365,31 +6365,31 @@
       </c>
       <c r="C78" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D78" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>마급</v>
       </c>
       <c r="E78" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F78" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G78" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>금융연구부</v>
       </c>
       <c r="H78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41058</v>
-      </c>
-      <c r="I78" s="1">
+        <v>40639</v>
+      </c>
+      <c r="I78" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>45818</v>
+        <v/>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -6399,7 +6399,7 @@
       </c>
       <c r="B79" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C79" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="D79" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>나급</v>
       </c>
       <c r="E79" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6423,7 +6423,7 @@
       </c>
       <c r="H79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43955</v>
+        <v>44487</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="B80" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C80" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6445,11 +6445,11 @@
       </c>
       <c r="D80" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E80" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F80" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6457,63 +6457,63 @@
       </c>
       <c r="G80" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>연구분석부</v>
       </c>
       <c r="H80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41966</v>
-      </c>
-      <c r="I80" s="1" t="str">
+        <v>43959</v>
+      </c>
+      <c r="I80" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>스위스</v>
+      </c>
+      <c r="C81" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>25569</v>
+      </c>
+      <c r="D81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>나급</v>
+      </c>
+      <c r="E81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>팀장</v>
+      </c>
+      <c r="G81" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>채권관리부</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>40888</v>
+      </c>
+      <c r="I81" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C81" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
-      </c>
-      <c r="D81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G81" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
-      </c>
-      <c r="H81" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>43507</v>
-      </c>
-      <c r="I81" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>45933</v>
-      </c>
-    </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B82" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C82" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6529,15 +6529,15 @@
       </c>
       <c r="F82" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G82" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40950</v>
+        <v>42564</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6551,7 +6551,7 @@
       </c>
       <c r="B83" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C83" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6559,11 +6559,11 @@
       </c>
       <c r="D83" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>다급</v>
       </c>
       <c r="E83" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F83" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6571,55 +6571,55 @@
       </c>
       <c r="G83" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>재산관리부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41153</v>
-      </c>
-      <c r="I83" s="1" t="str">
+        <v>41714</v>
+      </c>
+      <c r="I83" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>46196</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C84" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>라급</v>
+      </c>
+      <c r="E84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G84" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>재산관리부</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>42248</v>
+      </c>
+      <c r="I84" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
-      </c>
-      <c r="B84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
-      </c>
-      <c r="C84" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
-      </c>
-      <c r="D84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
-      </c>
-      <c r="E84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G84" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
-      </c>
-      <c r="H84" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44140</v>
-      </c>
-      <c r="I84" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>45190</v>
-      </c>
-    </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="B85" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C85" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6635,7 +6635,7 @@
       </c>
       <c r="D85" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>라급</v>
       </c>
       <c r="E85" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6651,7 +6651,7 @@
       </c>
       <c r="H85" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41105</v>
+        <v>41992</v>
       </c>
       <c r="I85" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6661,23 +6661,23 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C86" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>가급</v>
       </c>
       <c r="E86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6685,15 +6685,15 @@
       </c>
       <c r="G86" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>연구분석부</v>
       </c>
       <c r="H86" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43451</v>
-      </c>
-      <c r="I86" s="1" t="str">
+        <v>41212</v>
+      </c>
+      <c r="I86" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>46158</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -6707,7 +6707,7 @@
       </c>
       <c r="C87" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D87" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -6719,15 +6719,15 @@
       </c>
       <c r="F87" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G87" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>금융연구부</v>
       </c>
       <c r="H87" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41940</v>
+        <v>41102</v>
       </c>
       <c r="I87" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6737,19 +6737,19 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C88" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6757,15 +6757,15 @@
       </c>
       <c r="F88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G88" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>42060</v>
+        <v>43630</v>
       </c>
       <c r="I88" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6775,7 +6775,7 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B89" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6783,7 +6783,7 @@
       </c>
       <c r="C89" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D89" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -6795,15 +6795,15 @@
       </c>
       <c r="F89" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G89" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>연구분석부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41501</v>
+        <v>44287</v>
       </c>
       <c r="I89" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6821,11 +6821,11 @@
       </c>
       <c r="C90" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>25569</v>
       </c>
       <c r="D90" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>라급</v>
       </c>
       <c r="E90" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -6833,7 +6833,7 @@
       </c>
       <c r="F90" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G90" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>42549</v>
+        <v>40591</v>
       </c>
       <c r="I90" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6855,7 +6855,7 @@
       </c>
       <c r="B91" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
+        <v>한국</v>
       </c>
       <c r="C91" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
@@ -6863,11 +6863,11 @@
       </c>
       <c r="D91" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
+        <v>나급</v>
       </c>
       <c r="E91" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F91" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -6879,51 +6879,51 @@
       </c>
       <c r="H91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44150</v>
-      </c>
-      <c r="I91" s="1" t="str">
+        <v>41612</v>
+      </c>
+      <c r="I91" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>45271</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C92" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>29221</v>
+      </c>
+      <c r="D92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>라급</v>
+      </c>
+      <c r="E92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G92" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>재산관리부</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>41552</v>
+      </c>
+      <c r="I92" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
-      </c>
-      <c r="B92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
-      </c>
-      <c r="C92" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
-      </c>
-      <c r="D92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
-      </c>
-      <c r="E92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
-      </c>
-      <c r="G92" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
-      </c>
-      <c r="H92" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>41928</v>
-      </c>
-      <c r="I92" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>45501</v>
-      </c>
-    </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
@@ -6931,11 +6931,11 @@
       </c>
       <c r="B93" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C93" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>25569</v>
       </c>
       <c r="D93" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -6951,11 +6951,11 @@
       </c>
       <c r="G93" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43419</v>
+        <v>40846</v>
       </c>
       <c r="I93" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6965,7 +6965,7 @@
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -6977,27 +6977,27 @@
       </c>
       <c r="D94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>나급</v>
+        <v>다급</v>
       </c>
       <c r="E94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
+        <v>사원</v>
       </c>
       <c r="G94" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>채권관리부</v>
+        <v>재산관리부</v>
       </c>
       <c r="H94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>42790</v>
-      </c>
-      <c r="I94" s="1" t="str">
+        <v>41740</v>
+      </c>
+      <c r="I94" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>46331</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -7015,7 +7015,7 @@
       </c>
       <c r="D95" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>라급</v>
       </c>
       <c r="E95" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -7031,7 +7031,7 @@
       </c>
       <c r="H95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43675</v>
+        <v>43884</v>
       </c>
       <c r="I95" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="D96" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>가급</v>
+        <v>나급</v>
       </c>
       <c r="E96" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>42222</v>
+        <v>41001</v>
       </c>
       <c r="I96" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7079,15 +7079,15 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
+        <v>스위스</v>
       </c>
       <c r="C97" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
+        <v>29221</v>
       </c>
       <c r="D97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
@@ -7095,7 +7095,7 @@
       </c>
       <c r="E97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -7103,21 +7103,21 @@
       </c>
       <c r="G97" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>재산관리부</v>
       </c>
       <c r="H97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44393</v>
-      </c>
-      <c r="I97" s="1">
+        <v>41778</v>
+      </c>
+      <c r="I97" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>45262</v>
+        <v/>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>여</v>
+        <v>남</v>
       </c>
       <c r="B98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -7125,113 +7125,113 @@
       </c>
       <c r="C98" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
+        <v>29221</v>
       </c>
       <c r="D98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>마급</v>
+        <v>라급</v>
       </c>
       <c r="E98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>정규직</v>
+        <v>계약직</v>
       </c>
       <c r="F98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
+        <v>팀장</v>
       </c>
       <c r="G98" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>연구분석부</v>
       </c>
       <c r="H98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>43516</v>
-      </c>
-      <c r="I98" s="1" t="str">
+        <v>41808</v>
+      </c>
+      <c r="I98" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>46073</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C99" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>25569</v>
+      </c>
+      <c r="D99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>다급</v>
+      </c>
+      <c r="E99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>계약직</v>
+      </c>
+      <c r="F99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G99" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>홍보실</v>
+      </c>
+      <c r="H99" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>41286</v>
+      </c>
+      <c r="I99" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
+        <v>남</v>
+      </c>
+      <c r="B100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
+        <v>한국</v>
+      </c>
+      <c r="C100" s="1">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
+        <v>25569</v>
+      </c>
+      <c r="D100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
+        <v>나급</v>
+      </c>
+      <c r="E100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
+        <v>정규직</v>
+      </c>
+      <c r="F100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
+        <v>사원</v>
+      </c>
+      <c r="G100" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
+        <v>연구분석부</v>
+      </c>
+      <c r="H100" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>43372</v>
+      </c>
+      <c r="I100" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>한국</v>
-      </c>
-      <c r="C99" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>32874</v>
-      </c>
-      <c r="D99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
-      </c>
-      <c r="E99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>사원</v>
-      </c>
-      <c r="G99" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>금융연구부</v>
-      </c>
-      <c r="H99" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44267</v>
-      </c>
-      <c r="I99" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>45357</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
-      </c>
-      <c r="B100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
-        <v>스위스</v>
-      </c>
-      <c r="C100" s="1">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>25569</v>
-      </c>
-      <c r="D100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>다급</v>
-      </c>
-      <c r="E100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
-      </c>
-      <c r="F100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
-        <v>팀장</v>
-      </c>
-      <c r="G100" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
-      </c>
-      <c r="H100" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44023</v>
-      </c>
-      <c r="I100" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>46323</v>
-      </c>
-    </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3), lookup!$A$1:$B$3,2)</f>
-        <v>남</v>
+        <v>여</v>
       </c>
       <c r="B101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$C$1:$D$6,2)</f>
@@ -7239,15 +7239,15 @@
       </c>
       <c r="C101" s="1">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),lookup!$R$1:$S$6,2)</f>
-        <v>29221</v>
+        <v>32874</v>
       </c>
       <c r="D101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,10),lookup!$F$1:$G$10,2)</f>
-        <v>라급</v>
+        <v>다급</v>
       </c>
       <c r="E101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$I$1:$J$3,2)</f>
-        <v>계약직</v>
+        <v>정규직</v>
       </c>
       <c r="F101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,3),lookup!$L$1:$M$3,2)</f>
@@ -7255,15 +7255,15 @@
       </c>
       <c r="G101" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,5),lookup!$O$1:$P$5,2)</f>
-        <v>홍보실</v>
+        <v>채권관리부</v>
       </c>
       <c r="H101" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41505</v>
-      </c>
-      <c r="I101" s="1">
+        <v>43342</v>
+      </c>
+      <c r="I101" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>45530</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>